<commit_message>
Replace old MQTT timeout timer code to prevent stall condition. Introduced mqttRuntime function as solution.
</commit_message>
<xml_diff>
--- a/Support/S7 Symbols.xlsx
+++ b/Support/S7 Symbols.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>mqttAvailable</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>Data Type FB Number must match MQTT FB Number</t>
+  </si>
+  <si>
+    <t>mqttRuntime</t>
+  </si>
+  <si>
+    <t>FB      102</t>
   </si>
 </sst>
 </file>
@@ -513,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,186 +610,196 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection password="840F" sheet="1" objects="1" scenarios="1"/>
   <sortState ref="A1:C19">
     <sortCondition ref="B1:B19"/>
   </sortState>

</xml_diff>

<commit_message>
S7 Symbols.xlsx: added Unixtime and UDT_NET_CONFIG symbols
</commit_message>
<xml_diff>
--- a/Support/S7 Symbols.xlsx
+++ b/Support/S7 Symbols.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>mqttAvailable</t>
   </si>
@@ -157,6 +157,18 @@
   </si>
   <si>
     <t>FB      102</t>
+  </si>
+  <si>
+    <t>UDT_NET_CONFIG</t>
+  </si>
+  <si>
+    <t>UDT     101</t>
+  </si>
+  <si>
+    <t>Unixtime</t>
+  </si>
+  <si>
+    <t>FC     112</t>
   </si>
 </sst>
 </file>
@@ -519,11 +531,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -790,16 +800,40 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetProtection password="840F" sheet="1" objects="1" scenarios="1"/>
   <sortState ref="A1:C19">
     <sortCondition ref="B1:B19"/>
   </sortState>

</xml_diff>

<commit_message>
S7 Symbols.xlsx: fixed Symbols table duplicate symbol error
</commit_message>
<xml_diff>
--- a/Support/S7 Symbols.xlsx
+++ b/Support/S7 Symbols.xlsx
@@ -168,7 +168,7 @@
     <t>Unixtime</t>
   </si>
   <si>
-    <t>FC     112</t>
+    <t>FC     114</t>
   </si>
 </sst>
 </file>
@@ -533,7 +533,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>